<commit_message>
feat: add attendance, curriculum, schedule, and student management features
- Implemented AttendanceSummary and AttendanceTracker components.
- Created AttendanceContext for managing attendance state.
- Developed hooks for student filters and attendance services.
- Added types for attendance-related data structures.
- Established utility functions for attendance operations.
- Introduced curriculum components including CurriculumTab, LessonModal, and TemplateLibrary.
- Set up CurriculumContext and services for curriculum management.
- Defined types for curriculum data structures.
- Created CalendarGrid component for scheduling.
- Defined types for scheduled lessons.
- Implemented StudentsContext for managing student data with CRUD operations.
- Unified Student interface for consistent data handling across the application.
- Added router setup for application navigation.
</commit_message>
<xml_diff>
--- a/لوائح التلاميذ منفصلة/TCLSH-2.xlsx
+++ b/لوائح التلاميذ منفصلة/TCLSH-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30b93018d7010778/Documents/Classroom Management System/لوائح التلاميذ منفصلة/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabil\OneDrive\Documents\Classroom Management System\لوائح التلاميذ منفصلة\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{550F1E55-4ED6-4DAA-8D2B-1630EDF071B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63F22FC4-DE99-4BFE-9AEA-22DD12E0305A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951CAED6-D1D4-48D6-875C-AB11BA503D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B5EB18B5-8975-460C-A74A-965B97D6B6F5}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="134">
   <si>
     <t>ر.ت</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>2009-08-16</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -817,10 +820,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F191"/>
+  <dimension ref="A1:G191"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -837,7 +840,7 @@
     <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -857,7 +860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -877,7 +880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -897,7 +900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -916,8 +919,11 @@
       <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -937,7 +943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -957,7 +963,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -977,7 +983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -997,7 +1003,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1016,8 +1022,11 @@
       <c r="F9" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1037,7 +1046,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1057,7 +1066,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1077,7 +1086,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1097,7 +1106,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1117,7 +1126,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1137,7 +1146,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1155,6 +1164,9 @@
       </c>
       <c r="F16" s="4" t="s">
         <v>66</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>